<commit_message>
Updated the test date
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Playground\Workspace\LetShop\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC2893E-EFC9-465A-84D4-F00862DD078D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A893ECAD-5246-4EC0-BBFD-1A599E127D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Login</t>
   </si>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,7 +162,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +504,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE657D1D-E2FB-4BAB-8EEA-415327EF711F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0"/>
   </sheetViews>
@@ -534,18 +533,7 @@
       <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>